<commit_message>
added keywords and tests for new batch templates
</commit_message>
<xml_diff>
--- a/Testdata/PaymentsAndTransfers.xlsx
+++ b/Testdata/PaymentsAndTransfers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="13725" windowHeight="12945" tabRatio="500"/>
+    <workbookView windowWidth="28110" windowHeight="13095" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Maintain batch template" sheetId="1" r:id="rId1"/>
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
-  <si>
-    <t>Number</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="44">
+  <si>
+    <t>Position</t>
   </si>
   <si>
     <t>TemplateName</t>
@@ -38,6 +38,9 @@
     <t>OffsetAccount</t>
   </si>
   <si>
+    <t>a</t>
+  </si>
+  <si>
     <t>Ola_tp</t>
   </si>
   <si>
@@ -56,10 +59,19 @@
     <t>01110201 - Sacombank</t>
   </si>
   <si>
+    <t>b</t>
+  </si>
+  <si>
     <t>Partha_tp</t>
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
       <t xml:space="preserve">this is </t>
     </r>
     <r>
@@ -89,6 +101,9 @@
     <t>01110200 - checking</t>
   </si>
   <si>
+    <t>c</t>
+  </si>
+  <si>
     <t>Manikanta_tp</t>
   </si>
   <si>
@@ -101,6 +116,9 @@
     <t>01110101 - qqqq</t>
   </si>
   <si>
+    <t>d</t>
+  </si>
+  <si>
     <t>Ravikumar_tp</t>
   </si>
   <si>
@@ -110,12 +128,18 @@
     <t>01110100 - Justin Michael Pierson</t>
   </si>
   <si>
+    <t>e</t>
+  </si>
+  <si>
     <t>Anusha_tp</t>
   </si>
   <si>
     <t>this is E test template</t>
   </si>
   <si>
+    <t>f</t>
+  </si>
+  <si>
     <t>kandavelu_tp</t>
   </si>
   <si>
@@ -125,16 +149,25 @@
     <t>123456789 - BBTS TEST</t>
   </si>
   <si>
+    <t>g</t>
+  </si>
+  <si>
     <t>Priya_tp</t>
   </si>
   <si>
     <t>this is G test template</t>
   </si>
   <si>
+    <t>h</t>
+  </si>
+  <si>
     <t>stewagh_tp</t>
   </si>
   <si>
     <t>this is H test template</t>
+  </si>
+  <si>
+    <t>i</t>
   </si>
   <si>
     <t>lakshmi_tp</t>
@@ -148,10 +181,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -175,9 +208,91 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -189,142 +304,60 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -345,181 +378,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -554,50 +587,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -635,8 +629,47 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -654,138 +687,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1198,7 +1231,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54285714285714" defaultRowHeight="15" outlineLevelCol="6"/>
@@ -1237,210 +1270,210 @@
       </c>
     </row>
     <row r="2" customFormat="1" spans="1:7">
-      <c r="A2" s="4">
-        <v>1</v>
+      <c r="A2" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="1" spans="1:7">
-      <c r="A3" s="4">
-        <v>2</v>
+      <c r="A3" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="1" spans="1:7">
-      <c r="A4" s="4">
-        <v>3</v>
+      <c r="A4" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="1" spans="1:7">
-      <c r="A5" s="4">
-        <v>4</v>
+      <c r="A5" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="1" spans="1:7">
-      <c r="A6" s="4">
-        <v>5</v>
+      <c r="A6" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="1" spans="1:7">
-      <c r="A7" s="4">
-        <v>6</v>
+      <c r="A7" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="1" spans="1:7">
-      <c r="A8" s="4">
-        <v>7</v>
+      <c r="A8" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="1" spans="1:7">
-      <c r="A9" s="4">
-        <v>8</v>
+      <c r="A9" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="1" spans="1:7">
-      <c r="A10" s="4">
-        <v>9</v>
+      <c r="A10" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="3:4">

</xml_diff>

<commit_message>
changed keyword folder and updated tests and excel with alphanumeric
</commit_message>
<xml_diff>
--- a/Testdata/PaymentsAndTransfers.xlsx
+++ b/Testdata/PaymentsAndTransfers.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28110" windowHeight="13095" tabRatio="500"/>
+    <workbookView windowWidth="13725" windowHeight="12945" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Maintain batch template" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
     <t>OffsetAccount</t>
   </si>
   <si>
-    <t>a</t>
+    <t>TC01</t>
   </si>
   <si>
     <t>Ola_tp</t>
@@ -59,7 +59,7 @@
     <t>01110201 - Sacombank</t>
   </si>
   <si>
-    <t>b</t>
+    <t>TC02</t>
   </si>
   <si>
     <t>Partha_tp</t>
@@ -101,7 +101,7 @@
     <t>01110200 - checking</t>
   </si>
   <si>
-    <t>c</t>
+    <t>TC03</t>
   </si>
   <si>
     <t>Manikanta_tp</t>
@@ -116,7 +116,7 @@
     <t>01110101 - qqqq</t>
   </si>
   <si>
-    <t>d</t>
+    <t>TC04</t>
   </si>
   <si>
     <t>Ravikumar_tp</t>
@@ -128,7 +128,7 @@
     <t>01110100 - Justin Michael Pierson</t>
   </si>
   <si>
-    <t>e</t>
+    <t>TC05</t>
   </si>
   <si>
     <t>Anusha_tp</t>
@@ -137,7 +137,7 @@
     <t>this is E test template</t>
   </si>
   <si>
-    <t>f</t>
+    <t>TC06</t>
   </si>
   <si>
     <t>kandavelu_tp</t>
@@ -149,7 +149,7 @@
     <t>123456789 - BBTS TEST</t>
   </si>
   <si>
-    <t>g</t>
+    <t>TC07</t>
   </si>
   <si>
     <t>Priya_tp</t>
@@ -158,7 +158,7 @@
     <t>this is G test template</t>
   </si>
   <si>
-    <t>h</t>
+    <t>TC08</t>
   </si>
   <si>
     <t>stewagh_tp</t>
@@ -167,7 +167,7 @@
     <t>this is H test template</t>
   </si>
   <si>
-    <t>i</t>
+    <t>TC09</t>
   </si>
   <si>
     <t>lakshmi_tp</t>
@@ -181,9 +181,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
@@ -207,19 +207,20 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -227,8 +228,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -236,55 +274,38 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -297,13 +318,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -311,53 +325,39 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -378,187 +378,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -591,6 +591,15 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -612,6 +621,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -622,39 +646,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -676,6 +667,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -687,138 +687,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1231,7 +1231,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54285714285714" defaultRowHeight="15" outlineLevelCol="6"/>

</xml_diff>